<commit_message>
ANME and CommPhitting updates
</commit_message>
<xml_diff>
--- a/CommunityModeling/CommPhitting/data/Jeffs_data/metabolomics/8-19-22 Metabolomics TMS Panel EC_PF_acetate.xlsx
+++ b/CommunityModeling/CommPhitting/data/Jeffs_data/metabolomics/8-19-22 Metabolomics TMS Panel EC_PF_acetate.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Freiburger\Documents\Argonne\ProjectNotebooks\CommunityModeling\CommFitting\data\Jeffs_data\metabolomics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afreiburger/Documents/ProjectNotebooks/CommunityModeling/CommPhitting/data/Jeffs_data/metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF33E64-2077-724E-8169-BB2047EF1BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="11745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28280" windowHeight="18040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordered by Timepoint" sheetId="1" r:id="rId1"/>
     <sheet name="Ordered by condition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -267,7 +257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1219,7 +1209,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1227,6 +1216,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3597,7 +3587,7 @@
                   <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3854,7 +3844,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3862,6 +3851,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7809,7 +7799,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EABE569D-704D-EE4F-8B5B-DC4C4E272866}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7845,7 +7835,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29D62102-7A16-C047-9BDB-B035D10DCF65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7883,7 +7873,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{916620E7-16EB-9A4B-B7C0-A07579DFD810}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7921,7 +7911,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A40E335-27C5-9C40-84E5-63D6C8C875BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7959,7 +7949,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92056A18-ADE0-364D-934B-EB43EC924480}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7997,7 +7987,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6704B2F-A916-F344-8D00-8FCD33B34623}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8035,7 +8025,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EABE569D-704D-EE4F-8B5B-DC4C4E272866}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9784,16 +9774,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9831,7 +9821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -9869,7 +9859,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -9907,7 +9897,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -9945,7 +9935,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -9983,7 +9973,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -10021,7 +10011,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -10059,7 +10049,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -10097,7 +10087,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -10135,7 +10125,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -10173,7 +10163,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -10211,7 +10201,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -10249,7 +10239,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -10287,7 +10277,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -10325,7 +10315,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -10363,7 +10353,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -10401,7 +10391,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -10439,7 +10429,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -10477,7 +10467,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -10515,7 +10505,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -10553,7 +10543,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -10591,7 +10581,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -10629,7 +10619,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -10667,7 +10657,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -10705,7 +10695,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -10743,7 +10733,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -10781,7 +10771,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -10819,7 +10809,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -10857,7 +10847,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -10895,7 +10885,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -10933,7 +10923,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -10971,7 +10961,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -11009,19 +10999,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11038,7 +11028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -11055,7 +11045,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -11072,7 +11062,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -11089,7 +11079,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -11106,7 +11096,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -11123,7 +11113,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -11140,7 +11130,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -11157,7 +11147,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -11174,7 +11164,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -11191,7 +11181,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -11208,7 +11198,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -11225,7 +11215,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -11242,7 +11232,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -11259,7 +11249,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -11276,7 +11266,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -11293,7 +11283,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -11310,7 +11300,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -11327,7 +11317,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -11344,7 +11334,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -11361,7 +11351,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -11378,7 +11368,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -11395,7 +11385,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -11412,7 +11402,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -11429,7 +11419,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -11446,7 +11436,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -11463,7 +11453,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -11480,7 +11470,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -11497,7 +11487,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -11514,7 +11504,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -11531,7 +11521,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -11548,7 +11538,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G32" s="4" t="s">
         <v>76</v>
       </c>
@@ -11556,19 +11546,19 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="E34" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>42</v>
       </c>
@@ -11660,7 +11650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -11755,7 +11745,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -11772,10 +11762,10 @@
         <v>4</v>
       </c>
       <c r="F39" s="1">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -11870,7 +11860,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -11966,7 +11956,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
     <sortCondition ref="B2:B31"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>